<commit_message>
Changes for the ce configs
</commit_message>
<xml_diff>
--- a/cosmos_setup.xlsx
+++ b/cosmos_setup.xlsx
@@ -8,22 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\projects\python_trials\COSMOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9D4390-ABC4-45C6-8429-19A06DC78C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DDC292-431A-435B-99D8-44257D875CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{CAA57204-F970-41CE-B982-125D4D9700C4}"/>
+    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="17" xr2:uid="{CAA57204-F970-41CE-B982-125D4D9700C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Retailer" sheetId="1" r:id="rId1"/>
     <sheet name="EA_StatusUpdates" sheetId="5" r:id="rId2"/>
     <sheet name="MK_StatusUpdates" sheetId="6" r:id="rId3"/>
-    <sheet name="Checkout" sheetId="2" r:id="rId4"/>
-    <sheet name="Tabby" sheetId="7" r:id="rId5"/>
-    <sheet name="Tamara" sheetId="8" r:id="rId6"/>
-    <sheet name="Product" sheetId="3" r:id="rId7"/>
-    <sheet name="Inventory-SIOCS" sheetId="9" r:id="rId8"/>
-    <sheet name="Inventory-Farfetch" sheetId="10" r:id="rId9"/>
-    <sheet name="Inventory-SFCC" sheetId="4" r:id="rId10"/>
-    <sheet name="Inventory-RedAnt" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="13" r:id="rId5"/>
+    <sheet name="Checkout" sheetId="2" r:id="rId6"/>
+    <sheet name="Tabby" sheetId="7" r:id="rId7"/>
+    <sheet name="Tamara" sheetId="8" r:id="rId8"/>
+    <sheet name="Product" sheetId="3" r:id="rId9"/>
+    <sheet name="Inventory-SIOCS" sheetId="9" r:id="rId10"/>
+    <sheet name="Inventory-Farfetch" sheetId="10" r:id="rId11"/>
+    <sheet name="Inventory-SFCC" sheetId="4" r:id="rId12"/>
+    <sheet name="Inventory-RedAnt" sheetId="11" r:id="rId13"/>
+    <sheet name="CE" sheetId="14" r:id="rId14"/>
+    <sheet name="GeoCode" sheetId="20" r:id="rId15"/>
+    <sheet name="CEOrder" sheetId="15" r:id="rId16"/>
+    <sheet name="CEReturn" sheetId="16" r:id="rId17"/>
+    <sheet name="CEProduct" sheetId="17" r:id="rId18"/>
+    <sheet name="CEPrice" sheetId="19" r:id="rId19"/>
+    <sheet name="CEInventory" sheetId="18" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="177">
   <si>
     <t>Locations</t>
   </si>
@@ -357,18 +366,6 @@
     <t>SELECT count(DISTINCT SKU, Catalogue_REF, name_en, name_ar, VPN, images, 'online', sellable, link, barcodes, size, Color_Name,isReturnable, noOfDaysToReturn) as count FROM Tumi.Fluent_Products_vw where updated_at &gt;= :watermark</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>IzwXxln99LZHom+1dmEj3tsxJKPBf5+FtJYmhGoB0e84WE1qCdY7MPq9ZkkoSYQu</t>
   </si>
   <si>
@@ -451,6 +448,144 @@
   </si>
   <si>
     <t>wm9_storer</t>
+  </si>
+  <si>
+    <t>apiKey</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>deliveryChargeSku</t>
+  </si>
+  <si>
+    <t>filterCriteria</t>
+  </si>
+  <si>
+    <t>retailerId</t>
+  </si>
+  <si>
+    <t>tenderId</t>
+  </si>
+  <si>
+    <t>tenderType</t>
+  </si>
+  <si>
+    <t>Guess</t>
+  </si>
+  <si>
+    <t>?statuses=NEW&amp;statuses=IN_COMBI&amp;isAcknowledged=false&amp;page=1</t>
+  </si>
+  <si>
+    <t>CCARD</t>
+  </si>
+  <si>
+    <t>?statuses=IN_PROGRESS&amp;isAcknowledged=false&amp;page=1</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Guess_CE_OMS_P_D</t>
+  </si>
+  <si>
+    <t>WITH ranked_products AS (  SELECT SKU, ROW_NUMBER() OVER (PARTITION BY SKU ORDER BY updated_at DESC) AS rn FROM Guess.Channel_Engine_Products_vw WHERE details_price_code = 'AED' AND updated_at &gt;= :watermark ) SELECT COUNT(*) AS count FROM ranked_products WHERE rn = 1</t>
+  </si>
+  <si>
+    <t>productPriceId</t>
+  </si>
+  <si>
+    <t>Guess_CE_OMS_P_P_D</t>
+  </si>
+  <si>
+    <t>WITH ranked_products AS (SELECT SKU, name_en, name_ar, VPN, images, 0 details_price_code, 0 details_price_value, 0 details_discount_code, 0 details_discount_value, 0 price_after_discount_value, style, master_id, link, barcodes, size, Color_Name, category_trail, gender, kids_gender, long_description_en, long_description_ar, ROW_NUMBER() OVER (PARTITION BY SKU ORDER BY updated_at DESC) AS rn FROM  Guess.Channel_Engine_Products_vw WHERE details_price_code IN ('AED', 'SAR') AND updated_at &gt;= :watermark) SELECT SKU, name_en, name_ar, VPN, images, details_price_code, details_price_value,  details_discount_code, details_discount_value, price_after_discount_value, style, master_id, link, barcodes, size, Color_Name, category_trail, gender, kids_gender, long_description_en, long_description_ar FROM ranked_products WHERE rn = 1</t>
+  </si>
+  <si>
+    <t>sourceDetails_encrypted</t>
+  </si>
+  <si>
+    <t>mysql-clienteling-rds.cb808qsg6711.eu-west-2.rds.amazonaws.com</t>
+  </si>
+  <si>
+    <t>sourceDetails_mySqlUser</t>
+  </si>
+  <si>
+    <t>Mulesoft_Guess</t>
+  </si>
+  <si>
+    <t>WITH ranked_products AS ( SELECT SKU, name_en, details_price_code, details_price_value, details_discount_code, details_discount_value, price_after_discount_value, ROW_NUMBER() OVER (PARTITION BY SKU ORDER BY updated_at DESC) AS rn FROM Guess.Channel_Engine_Products_vw WHERE SKU IN (SKU_IDS)) SELECT SKU, name_en, details_price_code, details_price_value, details_discount_code, details_discount_value, price_after_discount_value FROM ranked_products WHERE rn = 1</t>
+  </si>
+  <si>
+    <t>GUESS_CE_Fluent_OMS_I_D</t>
+  </si>
+  <si>
+    <t>destinationDetails_encrypted</t>
+  </si>
+  <si>
+    <t>/chalhoub-channelengine-sapi/api/v1</t>
+  </si>
+  <si>
+    <t>offer/stock</t>
+  </si>
+  <si>
+    <t>destinationDetails_virtualLocationsForInventoryForAE</t>
+  </si>
+  <si>
+    <t>CE_guess</t>
+  </si>
+  <si>
+    <t>Nq/sbNCAHaKL/ZPvtuzSnp2pzXK5R+cqeSgTcMmFsNbyTUP/ljs3nGzfKZpiAVcy</t>
+  </si>
+  <si>
+    <t>guess-dev.channelengine.net</t>
+  </si>
+  <si>
+    <t>aNm3DYCCRP0rDio9U/J+o89bSAGfJdS3R1BLIX7YzhTgOe73ND5dq3FH5/1PF7HU</t>
+  </si>
+  <si>
+    <t>maps.googleapis.com</t>
+  </si>
+  <si>
+    <t>guess</t>
+  </si>
+  <si>
+    <t>GeoCoding_guess</t>
+  </si>
+  <si>
+    <t>CE_lacoste</t>
+  </si>
+  <si>
+    <t>lacoste</t>
+  </si>
+  <si>
+    <t>lacoste-dev.channelengine.net</t>
+  </si>
+  <si>
+    <t>GeoCoding_lacoste</t>
+  </si>
+  <si>
+    <t>asfasdfadsfasf</t>
+  </si>
+  <si>
+    <t>xpP7P47YCN+5gjm1VlD/3MS7bG1+IiDKWjv89+6rQclrfgGCE8AUpe7Qg+rpGX+X</t>
+  </si>
+  <si>
+    <t>CE_Guess_Order_Create</t>
+  </si>
+  <si>
+    <t>Trendyol.intAE_forwardCarriyoBooking</t>
+  </si>
+  <si>
+    <t>Trendyol.intAE_returnCarriyoBooking</t>
+  </si>
+  <si>
+    <t>Trendyol.intAE_salesTransferLocation</t>
+  </si>
+  <si>
+    <t>Trendyol.intAE_customerCarePhoneNumber</t>
+  </si>
+  <si>
+    <t>CE_Guess_Return_Create</t>
   </si>
 </sst>
 </file>
@@ -882,16 +1017,16 @@
         <v>1</v>
       </c>
       <c r="K1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="M1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="N1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1011,6 +1146,219 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EC70BA-01FF-44A7-B377-9C8A9D5A843A}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>32016</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>32019</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>32022</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>32023</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>32033</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFABA938-985C-461E-A480-79F1A074F11D}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2">
+        <v>443</v>
+      </c>
+      <c r="L2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>78</v>
+      </c>
+      <c r="R2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7FCC5A-6B42-4862-8980-B8AD62E98B29}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
@@ -1264,7 +1612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0803D3-D936-4C2C-B11F-8169C3B26D9F}">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -1396,6 +1744,482 @@
       </c>
       <c r="T2" t="s">
         <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71942E46-1B96-498E-BAD1-A54E62795C5F}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="68.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A0C1F1-4634-48DD-BED1-A3DB70FBF786}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4549AB9D-B7CE-4E21-B3D2-61DC73F10F3D}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J1" t="s">
+        <v>174</v>
+      </c>
+      <c r="K1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2">
+        <v>262513862236</v>
+      </c>
+      <c r="D2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2">
+        <v>67</v>
+      </c>
+      <c r="F2">
+        <v>3000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>45084</v>
+      </c>
+      <c r="K2">
+        <v>8005226783</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB73C0D0-BC34-4BE2-B8E8-E4DA06E1DB49}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0ED9B2-C97B-4F96-80AF-49C189BDB627}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N1" t="s">
+        <v>150</v>
+      </c>
+      <c r="O1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2">
+        <v>4000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K2" t="s">
+        <v>149</v>
+      </c>
+      <c r="M2">
+        <v>3306</v>
+      </c>
+      <c r="N2" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" s="2">
+        <v>45828.506284722222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA389582-EBAB-4BE4-BD92-1B55AA39BF2E}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2">
+        <v>4000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2">
+        <v>3306</v>
+      </c>
+      <c r="K2" t="s">
+        <v>151</v>
+      </c>
+      <c r="L2" s="2">
+        <v>45828.506284722222</v>
       </c>
     </row>
   </sheetData>
@@ -1478,11 +2302,150 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F10CA2B-EB28-408F-AAA8-426A42A019D2}">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
+        <v>157</v>
+      </c>
+      <c r="M1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" t="s">
+        <v>148</v>
+      </c>
+      <c r="T1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2">
+        <v>443</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>156</v>
+      </c>
+      <c r="N2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>77</v>
+      </c>
+      <c r="R2" t="s">
+        <v>78</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B4ED56-4AB5-4EDE-89F1-2CAC51076E89}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1556,11 +2519,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A696A4-895E-4F09-A728-41BBC0F5009B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD535E6C-DD5E-4EFF-AF34-E6FC3D1C48D7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8933440-D6CC-4ADD-8460-722F0C5A400F}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1627,7 +2614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6A35C1-446D-4448-8E83-1711FB8403C5}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1666,7 +2653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B4B5EA-2538-4BBB-BA36-51396C6B6726}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1714,7 +2701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68749C4-C0AF-4738-8380-F8595B92577E}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -1774,28 +2761,28 @@
         <v>56</v>
       </c>
       <c r="N1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O1" t="s">
         <v>7</v>
       </c>
       <c r="P1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q1" t="s">
+        <v>112</v>
+      </c>
+      <c r="R1" t="s">
+        <v>114</v>
+      </c>
+      <c r="S1" t="s">
         <v>116</v>
       </c>
-      <c r="R1" t="s">
-        <v>118</v>
-      </c>
-      <c r="S1" t="s">
-        <v>120</v>
-      </c>
       <c r="T1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="U1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="164.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1812,19 +2799,19 @@
         <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G2">
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J2" t="s">
         <v>87</v>
@@ -1833,247 +2820,34 @@
         <v>443</v>
       </c>
       <c r="L2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M2" t="s">
         <v>74</v>
       </c>
       <c r="N2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="P2" t="s">
         <v>15</v>
       </c>
       <c r="Q2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="R2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="S2">
         <v>3306</v>
       </c>
       <c r="T2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="U2" s="2">
         <v>45757.416898148149</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EC70BA-01FF-44A7-B377-9C8A9D5A843A}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>32016</v>
-      </c>
-      <c r="B2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>32019</v>
-      </c>
-      <c r="B3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>32022</v>
-      </c>
-      <c r="B4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>32023</v>
-      </c>
-      <c r="B5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>32033</v>
-      </c>
-      <c r="B6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFABA938-985C-461E-A480-79F1A074F11D}">
-  <dimension ref="A1:R2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>60</v>
-      </c>
-      <c r="R1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K2">
-        <v>443</v>
-      </c>
-      <c r="L2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M2" t="s">
-        <v>74</v>
-      </c>
-      <c r="N2" t="s">
-        <v>75</v>
-      </c>
-      <c r="O2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P2" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>78</v>
-      </c>
-      <c r="R2" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for the siocs inventory details
</commit_message>
<xml_diff>
--- a/cosmos_setup.xlsx
+++ b/cosmos_setup.xlsx
@@ -8,31 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\projects\python_trials\COSMOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DDC292-431A-435B-99D8-44257D875CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F4F49B-2025-4362-B72E-5F1BBA78027F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="17" xr2:uid="{CAA57204-F970-41CE-B982-125D4D9700C4}"/>
+    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{CAA57204-F970-41CE-B982-125D4D9700C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Retailer" sheetId="1" r:id="rId1"/>
     <sheet name="EA_StatusUpdates" sheetId="5" r:id="rId2"/>
     <sheet name="MK_StatusUpdates" sheetId="6" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="13" r:id="rId5"/>
-    <sheet name="Checkout" sheetId="2" r:id="rId6"/>
-    <sheet name="Tabby" sheetId="7" r:id="rId7"/>
-    <sheet name="Tamara" sheetId="8" r:id="rId8"/>
-    <sheet name="Product" sheetId="3" r:id="rId9"/>
-    <sheet name="Inventory-SIOCS" sheetId="9" r:id="rId10"/>
-    <sheet name="Inventory-Farfetch" sheetId="10" r:id="rId11"/>
-    <sheet name="Inventory-SFCC" sheetId="4" r:id="rId12"/>
-    <sheet name="Inventory-RedAnt" sheetId="11" r:id="rId13"/>
-    <sheet name="CE" sheetId="14" r:id="rId14"/>
-    <sheet name="GeoCode" sheetId="20" r:id="rId15"/>
-    <sheet name="CEOrder" sheetId="15" r:id="rId16"/>
-    <sheet name="CEReturn" sheetId="16" r:id="rId17"/>
-    <sheet name="CEProduct" sheetId="17" r:id="rId18"/>
-    <sheet name="CEPrice" sheetId="19" r:id="rId19"/>
-    <sheet name="CEInventory" sheetId="18" r:id="rId20"/>
+    <sheet name="Checkout" sheetId="2" r:id="rId4"/>
+    <sheet name="Tabby" sheetId="7" r:id="rId5"/>
+    <sheet name="Tamara" sheetId="8" r:id="rId6"/>
+    <sheet name="Product" sheetId="3" r:id="rId7"/>
+    <sheet name="Inventory-SIOCS" sheetId="9" r:id="rId8"/>
+    <sheet name="Inventory-Farfetch" sheetId="10" r:id="rId9"/>
+    <sheet name="Inventory-SFCC" sheetId="4" r:id="rId10"/>
+    <sheet name="Inventory-RedAnt" sheetId="11" r:id="rId11"/>
+    <sheet name="CE" sheetId="14" r:id="rId12"/>
+    <sheet name="GeoCode" sheetId="20" r:id="rId13"/>
+    <sheet name="CEOrder" sheetId="15" r:id="rId14"/>
+    <sheet name="CEReturn" sheetId="16" r:id="rId15"/>
+    <sheet name="CEProduct" sheetId="17" r:id="rId16"/>
+    <sheet name="CEPrice" sheetId="19" r:id="rId17"/>
+    <sheet name="CEInventory" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="175">
   <si>
     <t>Locations</t>
   </si>
@@ -417,21 +415,6 @@
     <t>watermark</t>
   </si>
   <si>
-    <t>Tumi_AE_FLUENT_32016_S_S_S</t>
-  </si>
-  <si>
-    <t>Tumi_AE_FLUENT_32019_S_S_S</t>
-  </si>
-  <si>
-    <t>Tumi_AE_FLUENT_32022_S_S_S</t>
-  </si>
-  <si>
-    <t>Tumi_AE_FLUENT_32023_S_S_S</t>
-  </si>
-  <si>
-    <t>Tumi_SA_FLUENT_32033_S_S_S</t>
-  </si>
-  <si>
     <t>fileProcessingDay</t>
   </si>
   <si>
@@ -450,6 +433,9 @@
     <t>wm9_storer</t>
   </si>
   <si>
+    <t>brand</t>
+  </si>
+  <si>
     <t>apiKey</t>
   </si>
   <si>
@@ -586,6 +572,12 @@
   </si>
   <si>
     <t>CE_Guess_Return_Create</t>
+  </si>
+  <si>
+    <t>Deal_AE_FLUENT_95001_S_S_S</t>
+  </si>
+  <si>
+    <t>Deal_AE_FLUENT</t>
   </si>
 </sst>
 </file>
@@ -970,7 +962,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,16 +1009,16 @@
         <v>1</v>
       </c>
       <c r="K1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="L1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="M1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="N1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1146,219 +1138,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EC70BA-01FF-44A7-B377-9C8A9D5A843A}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>32016</v>
-      </c>
-      <c r="B2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>32019</v>
-      </c>
-      <c r="B3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>32022</v>
-      </c>
-      <c r="B4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>32023</v>
-      </c>
-      <c r="B5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>32033</v>
-      </c>
-      <c r="B6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFABA938-985C-461E-A480-79F1A074F11D}">
-  <dimension ref="A1:R2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:S2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>60</v>
-      </c>
-      <c r="R1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K2">
-        <v>443</v>
-      </c>
-      <c r="L2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M2" t="s">
-        <v>74</v>
-      </c>
-      <c r="N2" t="s">
-        <v>75</v>
-      </c>
-      <c r="O2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P2" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>78</v>
-      </c>
-      <c r="R2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7FCC5A-6B42-4862-8980-B8AD62E98B29}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
@@ -1612,7 +1391,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0803D3-D936-4C2C-B11F-8169C3B26D9F}">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -1751,7 +1530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71942E46-1B96-498E-BAD1-A54E62795C5F}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1761,6 +1540,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="68.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1773,38 +1553,38 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
         <v>166</v>
       </c>
-      <c r="C3" t="s">
-        <v>170</v>
-      </c>
       <c r="D3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1812,7 +1592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A0C1F1-4634-48DD-BED1-A3DB70FBF786}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1833,38 +1613,38 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1872,7 +1652,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4549AB9D-B7CE-4E21-B3D2-61DC73F10F3D}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1894,45 +1674,45 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" t="s">
         <v>133</v>
       </c>
-      <c r="D1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" t="s">
-        <v>137</v>
-      </c>
       <c r="H1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="I1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2">
         <v>262513862236</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E2">
         <v>67</v>
@@ -1941,7 +1721,7 @@
         <v>3000</v>
       </c>
       <c r="G2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
@@ -1961,7 +1741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB73C0D0-BC34-4BE2-B8E8-E4DA06E1DB49}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -1970,6 +1750,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1979,42 +1762,42 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D2">
         <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -2028,12 +1811,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0ED9B2-C97B-4F96-80AF-49C189BDB627}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD27"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2063,13 +1846,13 @@
         <v>108</v>
       </c>
       <c r="G1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J1" t="s">
         <v>111</v>
@@ -2084,7 +1867,7 @@
         <v>116</v>
       </c>
       <c r="N1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="O1" t="s">
         <v>119</v>
@@ -2092,16 +1875,16 @@
     </row>
     <row r="2" spans="1:15" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B2">
         <v>4000</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E2" t="s">
         <v>74</v>
@@ -2110,25 +1893,25 @@
         <v>109</v>
       </c>
       <c r="G2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="M2">
         <v>3306</v>
       </c>
       <c r="N2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="O2" s="2">
         <v>45828.506284722222</v>
@@ -2139,15 +1922,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA389582-EBAB-4BE4-BD92-1B55AA39BF2E}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2166,7 +1952,7 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G1" t="s">
         <v>111</v>
@@ -2181,7 +1967,7 @@
         <v>116</v>
       </c>
       <c r="K1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L1" t="s">
         <v>119</v>
@@ -2189,37 +1975,179 @@
     </row>
     <row r="2" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B2">
         <v>4000</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
         <v>109</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J2">
         <v>3306</v>
       </c>
       <c r="K2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L2" s="2">
         <v>45828.506284722222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F10CA2B-EB28-408F-AAA8-426A42A019D2}">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" t="s">
+        <v>144</v>
+      </c>
+      <c r="T1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2">
+        <v>443</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>152</v>
+      </c>
+      <c r="N2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>77</v>
+      </c>
+      <c r="R2" t="s">
+        <v>78</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2295,145 +2223,6 @@
       </c>
       <c r="F4" t="b">
         <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F10CA2B-EB28-408F-AAA8-426A42A019D2}">
-  <dimension ref="A1:T2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" t="s">
-        <v>157</v>
-      </c>
-      <c r="M1" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" t="s">
-        <v>148</v>
-      </c>
-      <c r="T1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>155</v>
-      </c>
-      <c r="I2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J2" t="s">
-        <v>70</v>
-      </c>
-      <c r="K2">
-        <v>443</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>156</v>
-      </c>
-      <c r="N2" t="s">
-        <v>74</v>
-      </c>
-      <c r="O2" t="s">
-        <v>75</v>
-      </c>
-      <c r="P2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>77</v>
-      </c>
-      <c r="R2" t="s">
-        <v>78</v>
-      </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2519,30 +2308,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A696A4-895E-4F09-A728-41BBC0F5009B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD535E6C-DD5E-4EFF-AF34-E6FC3D1C48D7}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8933440-D6CC-4ADD-8460-722F0C5A400F}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2614,7 +2379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6A35C1-446D-4448-8E83-1711FB8403C5}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2653,7 +2418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B4B5EA-2538-4BBB-BA36-51396C6B6726}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2701,7 +2466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68749C4-C0AF-4738-8380-F8595B92577E}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -2853,4 +2618,180 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EC70BA-01FF-44A7-B377-9C8A9D5A843A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>95001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFABA938-985C-461E-A480-79F1A074F11D}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2">
+        <v>443</v>
+      </c>
+      <c r="L2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>78</v>
+      </c>
+      <c r="R2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes for the gift card config and retailer changes
</commit_message>
<xml_diff>
--- a/cosmos_setup.xlsx
+++ b/cosmos_setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\projects\python_trials\COSMOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F4F49B-2025-4362-B72E-5F1BBA78027F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BA6162-3C99-43E6-908D-CF230BE4B809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{CAA57204-F970-41CE-B982-125D4D9700C4}"/>
+    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{CAA57204-F970-41CE-B982-125D4D9700C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Retailer" sheetId="1" r:id="rId1"/>
@@ -53,17 +53,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="185">
   <si>
     <t>Locations</t>
   </si>
   <si>
-    <t>BrandName</t>
-  </si>
-  <si>
-    <t>SFSCCaseBrandName</t>
-  </si>
-  <si>
     <t>RedAnt</t>
   </si>
   <si>
@@ -88,18 +82,6 @@
     <t>tumi-sit-integration-user</t>
   </si>
   <si>
-    <t>Ecom ID</t>
-  </si>
-  <si>
-    <t>retailer_id</t>
-  </si>
-  <si>
-    <t>retailer_username</t>
-  </si>
-  <si>
-    <t>retailer_password</t>
-  </si>
-  <si>
     <t>Tumi</t>
   </si>
   <si>
@@ -578,6 +560,54 @@
   </si>
   <si>
     <t>Deal_AE_FLUENT</t>
+  </si>
+  <si>
+    <t>egcSku</t>
+  </si>
+  <si>
+    <t>epgcSku</t>
+  </si>
+  <si>
+    <t>egcPgmGroupName</t>
+  </si>
+  <si>
+    <t>egcCtryCode</t>
+  </si>
+  <si>
+    <t>ae</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>retailerUsername</t>
+  </si>
+  <si>
+    <t>retailerPwd</t>
+  </si>
+  <si>
+    <t>sfscCaseBrandName</t>
+  </si>
+  <si>
+    <t>TUMI KSA E-Gift Card</t>
+  </si>
+  <si>
+    <t>TUMI UAE E-Gift Card</t>
+  </si>
+  <si>
+    <t>EGIFT_107</t>
+  </si>
+  <si>
+    <t>EPGC_107</t>
+  </si>
+  <si>
+    <t>EcomLocations</t>
+  </si>
+  <si>
+    <t>egcLocations</t>
+  </si>
+  <si>
+    <t>epgcLocations</t>
   </si>
 </sst>
 </file>
@@ -619,12 +649,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112F64DB-7A09-4B36-A37A-D74421A9CF80}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,161 +1006,206 @@
     <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>175</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>177</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>182</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="L1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="M1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="N1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="O1" t="s">
+        <v>169</v>
+      </c>
+      <c r="P1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>172</v>
+      </c>
+      <c r="R1" t="s">
+        <v>171</v>
+      </c>
+      <c r="S1" t="s">
+        <v>170</v>
+      </c>
+      <c r="T1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
       </c>
       <c r="E2">
         <v>32016</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <v>32028</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="K2">
         <v>1000125</v>
       </c>
       <c r="L2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="O2" s="3">
+        <v>100000002005</v>
+      </c>
+      <c r="P2" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>173</v>
+      </c>
+      <c r="R2" t="s">
+        <v>179</v>
+      </c>
+      <c r="S2" s="3">
+        <v>100000002007</v>
+      </c>
+      <c r="T2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E3">
         <v>32019</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H3">
         <v>32029</v>
       </c>
       <c r="I3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <v>1000286</v>
       </c>
       <c r="L3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>174</v>
+      </c>
+      <c r="R3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E4">
         <v>32022</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H4">
         <v>32030</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E5">
         <v>32023</v>
       </c>
       <c r="F5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E6">
         <v>32034</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E7">
         <v>32031</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1156,233 +1232,233 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" t="s">
+      <c r="P1" t="s">
         <v>46</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
         <v>47</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>48</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>49</v>
       </c>
-      <c r="N1" t="s">
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="O1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
       </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="W1" t="s">
         <v>53</v>
       </c>
-      <c r="R1" t="s">
+      <c r="X1" t="s">
         <v>54</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Y1" t="s">
         <v>55</v>
-      </c>
-      <c r="T1" t="s">
-        <v>56</v>
-      </c>
-      <c r="U1" t="s">
-        <v>57</v>
-      </c>
-      <c r="V1" t="s">
-        <v>58</v>
-      </c>
-      <c r="W1" t="s">
-        <v>59</v>
-      </c>
-      <c r="X1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G2">
         <v>500</v>
       </c>
       <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" t="s">
         <v>65</v>
-      </c>
-      <c r="I2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J2" t="s">
-        <v>67</v>
-      </c>
-      <c r="K2" t="s">
-        <v>68</v>
-      </c>
-      <c r="L2" t="s">
-        <v>69</v>
-      </c>
-      <c r="M2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N2" t="s">
-        <v>71</v>
       </c>
       <c r="O2">
         <v>443</v>
       </c>
       <c r="P2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="Q2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" t="s">
         <v>67</v>
-      </c>
-      <c r="R2" t="s">
-        <v>73</v>
       </c>
       <c r="S2">
         <v>443</v>
       </c>
       <c r="T2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="U2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="V2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="W2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="X2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="Y2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C3">
         <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G3">
         <v>500</v>
       </c>
       <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" t="s">
         <v>65</v>
-      </c>
-      <c r="I3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K3" t="s">
-        <v>68</v>
-      </c>
-      <c r="L3" t="s">
-        <v>81</v>
-      </c>
-      <c r="M3" t="s">
-        <v>70</v>
-      </c>
-      <c r="N3" t="s">
-        <v>71</v>
       </c>
       <c r="O3">
         <v>443</v>
       </c>
       <c r="P3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="Q3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" t="s">
         <v>67</v>
-      </c>
-      <c r="R3" t="s">
-        <v>73</v>
       </c>
       <c r="S3">
         <v>444</v>
       </c>
       <c r="T3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="U3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="V3" t="s">
+        <v>70</v>
+      </c>
+      <c r="W3" t="s">
         <v>76</v>
       </c>
-      <c r="W3" t="s">
-        <v>82</v>
-      </c>
       <c r="X3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="Y3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1403,84 +1479,84 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" t="s">
-        <v>49</v>
-      </c>
       <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
-        <v>88</v>
-      </c>
-      <c r="O1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P1" t="s">
-        <v>57</v>
-      </c>
       <c r="Q1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="R1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="S1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="T1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G2">
         <v>500</v>
@@ -1492,37 +1568,37 @@
         <v>63034</v>
       </c>
       <c r="J2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="K2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="L2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="M2">
         <v>443</v>
       </c>
       <c r="N2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="O2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="P2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="Q2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="R2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="S2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="T2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1547,44 +1623,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1607,44 +1683,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1668,51 +1744,51 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="I1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="K1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C2">
         <v>262513862236</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E2">
         <v>67</v>
@@ -1721,7 +1797,7 @@
         <v>3000</v>
       </c>
       <c r="G2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
@@ -1756,48 +1832,48 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="H1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D2">
         <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -1828,90 +1904,90 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" t="s">
         <v>108</v>
       </c>
-      <c r="G1" t="s">
-        <v>141</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>144</v>
-      </c>
-      <c r="J1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L1" t="s">
-        <v>114</v>
-      </c>
       <c r="M1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="N1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="O1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B2">
         <v>4000</v>
       </c>
       <c r="C2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="K2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="M2">
         <v>3306</v>
       </c>
       <c r="N2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="O2" s="2">
         <v>45828.506284722222</v>
@@ -1937,72 +2013,72 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" t="s">
-        <v>114</v>
-      </c>
       <c r="J1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="L1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B2">
         <v>4000</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J2">
         <v>3306</v>
       </c>
       <c r="K2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="L2" s="2">
         <v>45828.506284722222</v>
@@ -2028,81 +2104,81 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
       <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>147</v>
+      </c>
+      <c r="M1" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" t="s">
         <v>51</v>
       </c>
-      <c r="L1" t="s">
-        <v>153</v>
-      </c>
-      <c r="M1" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O1" t="s">
-        <v>57</v>
-      </c>
       <c r="P1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="Q1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="R1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="S1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="T1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -2111,13 +2187,13 @@
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="I2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="K2">
         <v>443</v>
@@ -2126,28 +2202,28 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="N2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="O2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="P2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="Q2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="R2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="S2" t="b">
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2165,27 +2241,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2202,7 +2278,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -2219,7 +2295,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -2242,27 +2318,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -2279,7 +2355,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -2296,7 +2372,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -2325,53 +2401,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2391,26 +2467,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2430,35 +2506,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2487,129 +2563,129 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
       <c r="K1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="L1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="M1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="N1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>106</v>
+      </c>
+      <c r="R1" t="s">
         <v>108</v>
       </c>
-      <c r="O1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
+        <v>110</v>
+      </c>
+      <c r="T1" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" t="s">
-        <v>112</v>
-      </c>
-      <c r="R1" t="s">
-        <v>114</v>
-      </c>
-      <c r="S1" t="s">
-        <v>116</v>
-      </c>
-      <c r="T1" t="s">
-        <v>117</v>
-      </c>
       <c r="U1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="164.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G2">
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K2">
         <v>443</v>
       </c>
       <c r="L2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="P2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" t="s">
         <v>107</v>
       </c>
-      <c r="M2" t="s">
-        <v>74</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>109</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="P2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>113</v>
-      </c>
-      <c r="R2" t="s">
-        <v>115</v>
       </c>
       <c r="S2">
         <v>3306</v>
       </c>
       <c r="T2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="U2" s="2">
         <v>45757.416898148149</v>
@@ -2624,7 +2700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EC70BA-01FF-44A7-B377-9C8A9D5A843A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2638,16 +2714,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2655,13 +2731,13 @@
         <v>95001</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2681,114 +2757,114 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
       <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" t="s">
         <v>51</v>
       </c>
-      <c r="L1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N1" t="s">
-        <v>57</v>
-      </c>
       <c r="O1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="P1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="Q1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="R1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G2">
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K2">
         <v>443</v>
       </c>
       <c r="L2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="M2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="N2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="O2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="P2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="Q2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="R2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to accomodate multiple market places
</commit_message>
<xml_diff>
--- a/cosmos_setup.xlsx
+++ b/cosmos_setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\projects\python_trials\COSMOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BA6162-3C99-43E6-908D-CF230BE4B809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0BBD14-B3D2-4983-945E-7A2EE587ABD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{CAA57204-F970-41CE-B982-125D4D9700C4}"/>
+    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="7" activeTab="13" xr2:uid="{CAA57204-F970-41CE-B982-125D4D9700C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Retailer" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="192">
   <si>
     <t>Locations</t>
   </si>
@@ -608,6 +608,27 @@
   </si>
   <si>
     <t>epgcLocations</t>
+  </si>
+  <si>
+    <t>Amazon(v3).intAE_forwardCarriyoBooking</t>
+  </si>
+  <si>
+    <t>Trendyol.intAE_lineLevelDiscountField</t>
+  </si>
+  <si>
+    <t>Trendyol.intAE_orderLevelDiscountField</t>
+  </si>
+  <si>
+    <t>UNIT_DISCOUNT_AMOUNT</t>
+  </si>
+  <si>
+    <t>TOTAL_DISCOUNT_AMOUNT</t>
+  </si>
+  <si>
+    <t>Amazon(v3).intAE_lineLevelDiscountField</t>
+  </si>
+  <si>
+    <t>Amazon(v3).intAE_orderLevelDiscountField</t>
   </si>
 </sst>
 </file>
@@ -992,7 +1013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112F64DB-7A09-4B36-A37A-D74421A9CF80}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
@@ -1730,19 +1751,24 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4549AB9D-B7CE-4E21-B3D2-61DC73F10F3D}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1776,8 +1802,23 @@
       <c r="K1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>186</v>
+      </c>
+      <c r="M1" t="s">
+        <v>187</v>
+      </c>
+      <c r="N1" t="s">
+        <v>185</v>
+      </c>
+      <c r="O1" t="s">
+        <v>190</v>
+      </c>
+      <c r="P1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>161</v>
       </c>
@@ -1810,6 +1851,21 @@
       </c>
       <c r="K2">
         <v>8005226783</v>
+      </c>
+      <c r="L2" t="s">
+        <v>188</v>
+      </c>
+      <c r="M2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>188</v>
+      </c>
+      <c r="P2" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>